<commit_message>
updated vo names in stations. Updated all vehicle commands in editor
</commit_message>
<xml_diff>
--- a/01 Misc Modding Files/station_layout_planning.xlsx
+++ b/01 Misc Modding Files/station_layout_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\SteamLibrary\steamapps\common\911 First Responders\Mods\02_Reedy_Creek_Fire_Department_Mod\01 Misc Modding Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950BFFDC-A539-46CD-80DA-1E029AE06B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7414089-3958-4D22-94F1-DAC2905D3373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{7F1E8554-13DD-F343-A703-57B408EA4E60}"/>
+    <workbookView xWindow="3900" yWindow="2160" windowWidth="18270" windowHeight="13515" xr2:uid="{7F1E8554-13DD-F343-A703-57B408EA4E60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -526,7 +526,7 @@
   <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -678,14 +678,14 @@
         <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="8"/>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -693,14 +693,14 @@
         <v>25</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="8"/>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adjusted woods, both squads
</commit_message>
<xml_diff>
--- a/01 Misc Modding Files/station_layout_planning.xlsx
+++ b/01 Misc Modding Files/station_layout_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\SteamLibrary\steamapps\common\911 First Responders\Mods\02_Reedy_Creek_Fire_Department_Mod\01 Misc Modding Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7414089-3958-4D22-94F1-DAC2905D3373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32C3751-B3F0-429B-A5AB-F303A3C737B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2160" windowWidth="18270" windowHeight="13515" xr2:uid="{7F1E8554-13DD-F343-A703-57B408EA4E60}"/>
+    <workbookView xWindow="4455" yWindow="885" windowWidth="18270" windowHeight="13515" xr2:uid="{7F1E8554-13DD-F343-A703-57B408EA4E60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>Engine 31</t>
   </si>
   <si>
-    <t>Woods 31</t>
-  </si>
-  <si>
     <t>Rescue 31</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>1 (close to spawn)</t>
+  </si>
+  <si>
+    <t>Woods 32</t>
   </si>
 </sst>
 </file>
@@ -151,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +161,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -192,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -209,6 +215,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,7 +533,7 @@
   <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -542,13 +549,13 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -559,7 +566,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="3" t="s">
@@ -570,14 +577,12 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="7"/>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
+      <c r="C4" s="7"/>
+      <c r="D4" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -595,9 +600,11 @@
         <v>2</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
+      <c r="C5" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -613,8 +620,8 @@
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
+      <c r="D6" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -632,14 +639,14 @@
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
-        <v>10</v>
+      <c r="D7" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>12</v>
@@ -650,7 +657,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -659,10 +666,10 @@
         <v>11</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -675,7 +682,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -690,9 +697,9 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="8"/>
@@ -705,10 +712,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="C13" s="8"/>
       <c r="E13">
@@ -739,7 +746,7 @@
         <v>2</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -748,7 +755,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -761,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -769,7 +776,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated fire station start + added EMS captain to possible units to call
</commit_message>
<xml_diff>
--- a/01 Misc Modding Files/station_layout_planning.xlsx
+++ b/01 Misc Modding Files/station_layout_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Games\SteamLibrary\steamapps\common\911 First Responders\Mods\02_Reedy_Creek_Fire_Department_Mod\01 Misc Modding Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32C3751-B3F0-429B-A5AB-F303A3C737B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634A0240-C82A-4002-80F3-838DDAAB072C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="885" windowWidth="18270" windowHeight="13515" xr2:uid="{7F1E8554-13DD-F343-A703-57B408EA4E60}"/>
+    <workbookView xWindow="10185" yWindow="1020" windowWidth="18270" windowHeight="13515" xr2:uid="{7F1E8554-13DD-F343-A703-57B408EA4E60}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -166,7 +166,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,7 +533,7 @@
   <dimension ref="A2:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -562,10 +562,10 @@
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="6"/>
@@ -656,13 +656,13 @@
       <c r="A8" s="9">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -684,7 +684,7 @@
       <c r="A11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="8"/>

</xml_diff>